<commit_message>
Added a Do's and Don't list
</commit_message>
<xml_diff>
--- a/location-backend/locations.xlsx
+++ b/location-backend/locations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -46,6 +46,9 @@
     <t>First Sip Cafe</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>ChIJ33YxJNXTD4gRWe6jz5NdNpo</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>Bang Bang Pie &amp; Biscuits</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>ChIJt6mzLZ7SD4gR8bpjii62t_Q</t>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:N4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +475,20 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -501,19 +519,31 @@
       <c r="J2">
         <v>-87.6497045</v>
       </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <v>41.9489773</v>
+      </c>
+      <c r="N2">
+        <v>-87.6497045</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>41.9731758</v>
@@ -522,10 +552,10 @@
         <v>-87.6572092</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3">
         <v>41.9731758</v>
@@ -533,19 +563,31 @@
       <c r="J3">
         <v>-87.6572092</v>
       </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3">
+        <v>41.9731758</v>
+      </c>
+      <c r="N3">
+        <v>-87.6572092</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>41.9190202</v>
@@ -554,15 +596,27 @@
         <v>-87.6971201</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>41.9190202</v>
       </c>
       <c r="J4">
+        <v>-87.6971201</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4">
+        <v>41.9190202</v>
+      </c>
+      <c r="N4">
         <v>-87.6971201</v>
       </c>
     </row>

</xml_diff>